<commit_message>
GoodInfo_v2 - 2021.11.22 完成
</commit_message>
<xml_diff>
--- a/GoodInfo_StockList_20211119.xlsx
+++ b/GoodInfo_StockList_20211119.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>代號</t>
   </si>
@@ -39,15 +39,9 @@
     <t>大量_小計</t>
   </si>
   <si>
-    <t>merge_status</t>
-  </si>
-  <si>
     <t>南亞</t>
   </si>
   <si>
-    <t>both</t>
-  </si>
-  <si>
     <t>中電</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
   </si>
   <si>
     <t>聯電</t>
-  </si>
-  <si>
-    <t>left_only</t>
   </si>
   <si>
     <t>光罩</t>
@@ -583,15 +574,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -613,11 +604,8 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -625,7 +613,7 @@
         <v>1303</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -633,11 +621,8 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -645,7 +630,7 @@
         <v>1611</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>4.22</v>
@@ -653,11 +638,8 @@
       <c r="H3">
         <v>4.22</v>
       </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -665,7 +647,7 @@
         <v>1709</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>2.5</v>
@@ -676,11 +658,8 @@
       <c r="H4">
         <v>2.2400000000000002</v>
       </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -688,7 +667,7 @@
         <v>1722</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -702,11 +681,8 @@
       <c r="H5">
         <v>22.82</v>
       </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -714,7 +690,7 @@
         <v>1810</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>2.5</v>
@@ -725,11 +701,8 @@
       <c r="H6">
         <v>3.39</v>
       </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -737,13 +710,10 @@
         <v>2303</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -751,7 +721,7 @@
         <v>2338</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -762,11 +732,8 @@
       <c r="H8">
         <v>10.44</v>
       </c>
-      <c r="I8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -774,7 +741,7 @@
         <v>2340</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -785,11 +752,8 @@
       <c r="H9">
         <v>3.84</v>
       </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -797,7 +761,7 @@
         <v>2374</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10">
         <v>4.55</v>
@@ -805,11 +769,8 @@
       <c r="H10">
         <v>4.55</v>
       </c>
-      <c r="I10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -817,7 +778,7 @@
         <v>2376</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>0.85</v>
@@ -828,11 +789,8 @@
       <c r="H11">
         <v>10.57</v>
       </c>
-      <c r="I11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -840,7 +798,7 @@
         <v>2436</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -854,11 +812,8 @@
       <c r="H12">
         <v>6.7799999999999994</v>
       </c>
-      <c r="I12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -866,13 +821,10 @@
         <v>2455</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -880,7 +832,7 @@
         <v>2476</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -894,11 +846,8 @@
       <c r="H14">
         <v>23.94</v>
       </c>
-      <c r="I14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -906,7 +855,7 @@
         <v>2484</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -917,11 +866,8 @@
       <c r="H15">
         <v>3.84</v>
       </c>
-      <c r="I15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -929,7 +875,7 @@
         <v>2610</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -940,11 +886,8 @@
       <c r="H16">
         <v>3.37</v>
       </c>
-      <c r="I16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -952,7 +895,7 @@
         <v>2618</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>6.75</v>
@@ -960,11 +903,8 @@
       <c r="H17">
         <v>6.75</v>
       </c>
-      <c r="I17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -972,7 +912,7 @@
         <v>3016</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -983,11 +923,8 @@
       <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -995,7 +932,7 @@
         <v>3017</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1012,11 +949,8 @@
       <c r="H19">
         <v>37.270000000000003</v>
       </c>
-      <c r="I19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1024,7 +958,7 @@
         <v>3037</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <v>2.2999999999999998</v>
@@ -1038,11 +972,8 @@
       <c r="H20">
         <v>11.57</v>
       </c>
-      <c r="I20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1050,7 +981,7 @@
         <v>3041</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D21">
         <v>2.5</v>
@@ -1061,11 +992,8 @@
       <c r="H21">
         <v>16.25</v>
       </c>
-      <c r="I21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1073,7 +1001,7 @@
         <v>3062</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -1084,11 +1012,8 @@
       <c r="H22">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1096,7 +1021,7 @@
         <v>3122</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D23">
         <v>2.9</v>
@@ -1110,11 +1035,8 @@
       <c r="H23">
         <v>12.34</v>
       </c>
-      <c r="I23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1122,7 +1044,7 @@
         <v>3169</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D24">
         <v>2.5</v>
@@ -1136,11 +1058,8 @@
       <c r="H24">
         <v>6.71</v>
       </c>
-      <c r="I24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1148,7 +1067,7 @@
         <v>3189</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -1162,11 +1081,8 @@
       <c r="H25">
         <v>20.69</v>
       </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1174,7 +1090,7 @@
         <v>3305</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E26">
         <v>2.02</v>
@@ -1185,11 +1101,8 @@
       <c r="H26">
         <v>7.69</v>
       </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1197,7 +1110,7 @@
         <v>3491</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -1211,11 +1124,8 @@
       <c r="H27">
         <v>14.69</v>
       </c>
-      <c r="I27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1223,7 +1133,7 @@
         <v>3504</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -1237,11 +1147,8 @@
       <c r="H28">
         <v>22.97</v>
       </c>
-      <c r="I28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1249,7 +1156,7 @@
         <v>3515</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E29">
         <v>4.17</v>
@@ -1257,11 +1164,8 @@
       <c r="H29">
         <v>4.17</v>
       </c>
-      <c r="I29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1269,7 +1173,7 @@
         <v>3588</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1283,11 +1187,8 @@
       <c r="H30">
         <v>8.18</v>
       </c>
-      <c r="I30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1295,13 +1196,10 @@
         <v>3596</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="I31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1309,7 +1207,7 @@
         <v>4721</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D32">
         <v>2.9</v>
@@ -1323,11 +1221,8 @@
       <c r="H32">
         <v>15.75</v>
       </c>
-      <c r="I32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1335,7 +1230,7 @@
         <v>4927</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D33">
         <v>2.2999999999999998</v>
@@ -1346,11 +1241,8 @@
       <c r="H33">
         <v>4.8899999999999997</v>
       </c>
-      <c r="I33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1358,7 +1250,7 @@
         <v>5227</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E34">
         <v>7.94</v>
@@ -1366,11 +1258,8 @@
       <c r="H34">
         <v>7.94</v>
       </c>
-      <c r="I34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1378,7 +1267,7 @@
         <v>5258</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -1392,11 +1281,8 @@
       <c r="H35">
         <v>19.62</v>
       </c>
-      <c r="I35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1404,7 +1290,7 @@
         <v>5351</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1415,11 +1301,8 @@
       <c r="H36">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1427,7 +1310,7 @@
         <v>5371</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E37">
         <v>2.3199999999999998</v>
@@ -1438,11 +1321,8 @@
       <c r="H37">
         <v>11.37</v>
       </c>
-      <c r="I37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1450,7 +1330,7 @@
         <v>6104</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -1461,11 +1341,8 @@
       <c r="H38">
         <v>3.65</v>
       </c>
-      <c r="I38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1473,7 +1350,7 @@
         <v>6118</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -1484,11 +1361,8 @@
       <c r="H39">
         <v>3.12</v>
       </c>
-      <c r="I39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1496,7 +1370,7 @@
         <v>6138</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -1507,11 +1381,8 @@
       <c r="H40">
         <v>3.45</v>
       </c>
-      <c r="I40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1519,13 +1390,10 @@
         <v>6143</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
-      </c>
-      <c r="I41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1533,13 +1401,10 @@
         <v>6167</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
-      </c>
-      <c r="I42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1547,7 +1412,7 @@
         <v>6191</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -1558,11 +1423,8 @@
       <c r="H43">
         <v>3.42</v>
       </c>
-      <c r="I43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1570,7 +1432,7 @@
         <v>6196</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D44">
         <v>2.9</v>
@@ -1584,11 +1446,8 @@
       <c r="H44">
         <v>15.46</v>
       </c>
-      <c r="I44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1596,7 +1455,7 @@
         <v>6265</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D45">
         <v>2.5</v>
@@ -1607,11 +1466,8 @@
       <c r="H45">
         <v>2.76</v>
       </c>
-      <c r="I45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1619,7 +1475,7 @@
         <v>6271</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D46">
         <v>2.2999999999999998</v>
@@ -1630,11 +1486,8 @@
       <c r="H46">
         <v>3.77</v>
       </c>
-      <c r="I46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1642,7 +1495,7 @@
         <v>6282</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -1656,11 +1509,8 @@
       <c r="H47">
         <v>27.16</v>
       </c>
-      <c r="I47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1668,7 +1518,7 @@
         <v>6457</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E48">
         <v>7.26</v>
@@ -1676,11 +1526,8 @@
       <c r="H48">
         <v>7.26</v>
       </c>
-      <c r="I48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1688,7 +1535,7 @@
         <v>6533</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D49">
         <v>2</v>
@@ -1702,11 +1549,8 @@
       <c r="H49">
         <v>10.08</v>
       </c>
-      <c r="I49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1714,7 +1558,7 @@
         <v>8046</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -1728,11 +1572,8 @@
       <c r="H50">
         <v>6.01</v>
       </c>
-      <c r="I50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1740,7 +1581,7 @@
         <v>8069</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D51">
         <v>3</v>
@@ -1751,11 +1592,8 @@
       <c r="H51">
         <v>0.7</v>
       </c>
-      <c r="I51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1763,7 +1601,7 @@
         <v>8103</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D52">
         <v>2.5</v>
@@ -1774,11 +1612,8 @@
       <c r="H52">
         <v>1.67</v>
       </c>
-      <c r="I52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1786,7 +1621,7 @@
         <v>8182</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D53">
         <v>3</v>
@@ -1800,11 +1635,8 @@
       <c r="H53">
         <v>5.88</v>
       </c>
-      <c r="I53" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1812,7 +1644,7 @@
         <v>8201</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E54">
         <v>14.95</v>
@@ -1820,11 +1652,8 @@
       <c r="H54">
         <v>14.95</v>
       </c>
-      <c r="I54" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1832,7 +1661,7 @@
         <v>8289</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -1842,9 +1671,6 @@
       </c>
       <c r="H55">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="I55" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>